<commit_message>
modif script creation bdd + mcd + jeu de donnees
</commit_message>
<xml_diff>
--- a/Fil_Rouge/jeu_de_donnees/jeu_de_donnees_village_green.xlsx
+++ b/Fil_Rouge/jeu_de_donnees/jeu_de_donnees_village_green.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,21 +14,22 @@
     <sheet name="clients" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="commandes" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="livre" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="paie" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="reglements" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="produits" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="contient" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="tva" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="fournisseurs" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="founi" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="rubriques" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="reglements" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="paie" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="rubriques" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="produits" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="fournisseurs" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="fourni" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="contient" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="tva" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="applique" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>libRole</t>
   </si>
@@ -202,12 +203,204 @@
   </si>
   <si>
     <t>4e6fs</t>
+  </si>
+  <si>
+    <t>numCommande</t>
+  </si>
+  <si>
+    <t>dateCommande</t>
+  </si>
+  <si>
+    <t>dateCommandeFormat</t>
+  </si>
+  <si>
+    <t>idClientManuel</t>
+  </si>
+  <si>
+    <t>idCommande</t>
+  </si>
+  <si>
+    <t>dateLivraison</t>
+  </si>
+  <si>
+    <t>dateLivraisonFormat</t>
+  </si>
+  <si>
+    <t>quantiteLivraison</t>
+  </si>
+  <si>
+    <t>idLivre</t>
+  </si>
+  <si>
+    <t>typePaiement</t>
+  </si>
+  <si>
+    <t>idReglement</t>
+  </si>
+  <si>
+    <t>Différé</t>
+  </si>
+  <si>
+    <t>Comptant</t>
+  </si>
+  <si>
+    <t>Reglement</t>
+  </si>
+  <si>
+    <t>datePaiement</t>
+  </si>
+  <si>
+    <t>datePaiementFormat</t>
+  </si>
+  <si>
+    <t>montantPaiement</t>
+  </si>
+  <si>
+    <t>idPaie</t>
+  </si>
+  <si>
+    <t>libRubrique</t>
+  </si>
+  <si>
+    <t>idRubrique</t>
+  </si>
+  <si>
+    <t>idRubrique_1</t>
+  </si>
+  <si>
+    <t>jouets</t>
+  </si>
+  <si>
+    <t>meubles</t>
+  </si>
+  <si>
+    <t>outils</t>
+  </si>
+  <si>
+    <t>electromenager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meubles de bureau</t>
+  </si>
+  <si>
+    <t>libProduit</t>
+  </si>
+  <si>
+    <t>descProduit</t>
+  </si>
+  <si>
+    <t>refProduit</t>
+  </si>
+  <si>
+    <t>prixProduit</t>
+  </si>
+  <si>
+    <t>photoProduit</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>Rubrique</t>
+  </si>
+  <si>
+    <t>idProduit</t>
+  </si>
+  <si>
+    <t>chaise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chaise très confortable</t>
+  </si>
+  <si>
+    <t>f7s9e</t>
+  </si>
+  <si>
+    <t>poupée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poupée parfaite comme cadeau d'anniversaire ou de noël</t>
+  </si>
+  <si>
+    <t>h8d7g</t>
+  </si>
+  <si>
+    <t>../IMG/poupee.png</t>
+  </si>
+  <si>
+    <t>tournevis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tournevis parfait pour vos tâches du quotidien</t>
+  </si>
+  <si>
+    <t>c8s23</t>
+  </si>
+  <si>
+    <t>canapé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">canapé très confortable</t>
+  </si>
+  <si>
+    <t>h8sdg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">machine à laver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">machine à laver parfaite pour vos vêtements</t>
+  </si>
+  <si>
+    <t>d8g3d</t>
+  </si>
+  <si>
+    <t>nomFournisseur</t>
+  </si>
+  <si>
+    <t>idFournisseur</t>
+  </si>
+  <si>
+    <t>SuperElectro</t>
+  </si>
+  <si>
+    <t>SuperMaison</t>
+  </si>
+  <si>
+    <t>SuperJouets</t>
+  </si>
+  <si>
+    <t>idFourni</t>
+  </si>
+  <si>
+    <t>quantiteProduit</t>
+  </si>
+  <si>
+    <t>idContient</t>
+  </si>
+  <si>
+    <t>tauxTva</t>
+  </si>
+  <si>
+    <t>idTva</t>
+  </si>
+  <si>
+    <t>dateTva</t>
+  </si>
+  <si>
+    <t>dateTvaFormat</t>
+  </si>
+  <si>
+    <t>idApplique</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="160" formatCode="dd/mm/yyyy"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <name val="Calibri"/>
@@ -352,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="29">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -366,11 +559,47 @@
     <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="2" fillId="0" borderId="7" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="7" numFmtId="160" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="7" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="7" numFmtId="160" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="1" fillId="0" borderId="7" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="7" numFmtId="160" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -959,8 +1188,177 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="11.8515625"/>
+    <col bestFit="1" min="2" max="2" width="10.2109375"/>
+    <col bestFit="1" min="3" max="3" width="12.421875"/>
+    <col bestFit="1" min="4" max="4" width="14.78125"/>
+    <col bestFit="1" min="5" max="5" width="13.00390625"/>
+    <col bestFit="1" min="6" max="6" width="19.2109375"/>
+    <col bestFit="1" min="7" max="7" width="16.640625"/>
+    <col bestFit="1" min="10" max="10" width="113.640625"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="10">
+        <f>VLOOKUP(B2,reglements!$A$2:$B$3,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="10">
+        <f>VLOOKUP(D2,commandes!$A$2:$I$5,9,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D2" s="10">
+        <v>7824938248</v>
+      </c>
+      <c r="E2" s="16">
+        <v>44395</v>
+      </c>
+      <c r="F2" s="16" t="str">
+        <f>TEXT(E2,"aaaa-mm-jj")</f>
+        <v>-07-jj</v>
+      </c>
+      <c r="G2" s="10">
+        <v>80</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1</v>
+      </c>
+      <c r="J2" t="str">
+        <f>"INSERT INTO paie(idReglement, idCommande, datePaiement, montantPaiement) VALUES ("&amp;A2&amp;","&amp;C2&amp;","""&amp;F2&amp;""","&amp;G2&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO paie(idReglement, idCommande, datePaiement, montantPaiement) VALUES (2,2,"-07-jj",80);</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="10">
+        <f>VLOOKUP(B3,reglements!$A$2:$B$3,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="10">
+        <f>VLOOKUP(D3,commandes!$A$2:$I$5,9,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1579875647</v>
+      </c>
+      <c r="E3" s="16">
+        <v>44896</v>
+      </c>
+      <c r="F3" s="20" t="str">
+        <f>TEXT(E3,"aaaa-mm-jj")</f>
+        <v>-12-jj</v>
+      </c>
+      <c r="G3" s="10">
+        <v>758</v>
+      </c>
+      <c r="H3" s="10">
+        <v>2</v>
+      </c>
+      <c r="J3" t="str">
+        <f>"INSERT INTO paie(idReglement, idCommande, datePaiement, montantPaiement) VALUES ("&amp;A3&amp;","&amp;C3&amp;","""&amp;F3&amp;""","&amp;G3&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO paie(idReglement, idCommande, datePaiement, montantPaiement) VALUES (1,1,"-12-jj",758);</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="10">
+        <f>VLOOKUP(B4,reglements!$A$2:$B$3,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="10">
+        <f>VLOOKUP(D4,commandes!$A$2:$I$5,9,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D4" s="10">
+        <v>9854673485</v>
+      </c>
+      <c r="E4" s="16">
+        <v>43958</v>
+      </c>
+      <c r="F4" s="20" t="str">
+        <f>TEXT(E4,"aaaa-mm-jj")</f>
+        <v>-05-jj</v>
+      </c>
+      <c r="G4" s="10">
+        <v>465</v>
+      </c>
+      <c r="H4" s="10">
+        <v>3</v>
+      </c>
+      <c r="J4" t="str">
+        <f>"INSERT INTO paie(idReglement, idCommande, datePaiement, montantPaiement) VALUES ("&amp;A4&amp;","&amp;C4&amp;","""&amp;F4&amp;""","&amp;G4&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO paie(idReglement, idCommande, datePaiement, montantPaiement) VALUES (1,3,"-05-jj",465);</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="10">
+        <f>VLOOKUP(B5,reglements!$A$2:$B$3,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="10">
+        <f>VLOOKUP(D5,commandes!$A$2:$I$5,9,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="D5" s="10">
+        <v>4723541584</v>
+      </c>
+      <c r="E5" s="16">
+        <v>44608</v>
+      </c>
+      <c r="F5" s="20" t="str">
+        <f>TEXT(E5,"aaaa-mm-jj")</f>
+        <v>-02-jj</v>
+      </c>
+      <c r="G5" s="10">
+        <v>55</v>
+      </c>
+      <c r="H5" s="10">
+        <v>4</v>
+      </c>
+      <c r="J5" t="str">
+        <f>"INSERT INTO paie(idReglement, idCommande, datePaiement, montantPaiement) VALUES ("&amp;A5&amp;","&amp;C5&amp;","""&amp;F5&amp;""","&amp;G5&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO paie(idReglement, idCommande, datePaiement, montantPaiement) VALUES (2,4,"-02-jj",55);</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -975,8 +1373,89 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="17.07421875"/>
+    <col bestFit="1" min="2" max="2" width="10.421875"/>
+    <col bestFit="1" min="3" max="3" width="12.57421875"/>
+    <col bestFit="1" min="5" max="5" width="72.921875"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"INSERT INTO Rubriques(libRubrique, idRubrique_1) VALUES ("""&amp;A2&amp;""","&amp;C2&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO Rubriques(libRubrique, idRubrique_1) VALUES ("jouets",);</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="str">
+        <f>"INSERT INTO Rubriques(libRubrique, idRubrique_1) VALUES ("""&amp;A3&amp;""","&amp;C3&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO Rubriques(libRubrique, idRubrique_1) VALUES ("meubles",);</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="str">
+        <f>"INSERT INTO Rubriques(libRubrique, idRubrique_1) VALUES ("""&amp;A4&amp;""","&amp;C4&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO Rubriques(libRubrique, idRubrique_1) VALUES ("outils",);</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="str">
+        <f>"INSERT INTO Rubriques(libRubrique, idRubrique_1) VALUES ("""&amp;A5&amp;""","&amp;C5&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO Rubriques(libRubrique, idRubrique_1) VALUES ("electromenager",);</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="str">
+        <f>"INSERT INTO Rubriques(libRubrique, idRubrique_1) VALUES ("""&amp;A6&amp;""","&amp;C6&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO Rubriques(libRubrique, idRubrique_1) VALUES ("meubles de bureau",2);</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -991,8 +1470,212 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="14.140625"/>
+    <col bestFit="1" min="2" max="2" width="20.921875"/>
+    <col bestFit="1" min="3" max="3" width="9.640625"/>
+    <col bestFit="1" min="4" max="4" width="10.50390625"/>
+    <col bestFit="1" min="5" max="5" width="12.50390625"/>
+    <col bestFit="1" min="6" max="6" width="5.28125"/>
+    <col bestFit="1" min="7" max="7" width="10.421875"/>
+    <col bestFit="1" min="8" max="8" width="17.07421875"/>
+    <col bestFit="1" min="9" max="9" width="8.8515625"/>
+    <col bestFit="1" min="11" max="11" width="190.00390625"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="23">
+        <v>30</v>
+      </c>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23">
+        <v>20</v>
+      </c>
+      <c r="G2" s="23">
+        <f>VLOOKUP(H2,rubriques!$A$2:$C$6,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" s="23">
+        <v>1</v>
+      </c>
+      <c r="K2" t="str">
+        <f>"INSERT INTO Produits(libProduit, descProduit, refProduit, prixProduit, photoProduit, stock, idRubrique) VALUES ("""&amp;A2&amp;""","""&amp;B2&amp;""","""&amp;C2&amp;""","&amp;D2&amp;","""&amp;E2&amp;""","&amp;F2&amp;","&amp;G2&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO Produits(libProduit, descProduit, refProduit, prixProduit, photoProduit, stock, idRubrique) VALUES ("chaise","chaise très confortable","f7s9e",30,"",20,5);</v>
+      </c>
+    </row>
+    <row r="3" ht="57">
+      <c r="A3" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="23">
+        <v>15</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="23">
+        <v>150</v>
+      </c>
+      <c r="G3" s="23">
+        <f>VLOOKUP(H3,rubriques!$A$2:$C$6,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3" s="23">
+        <v>2</v>
+      </c>
+      <c r="K3" t="str">
+        <f>"INSERT INTO Produits(libProduit, descProduit, refProduit, prixProduit, photoProduit, stock, idRubrique) VALUES ("""&amp;A3&amp;""","""&amp;B3&amp;""","""&amp;C3&amp;""","&amp;D3&amp;","""&amp;E3&amp;""","&amp;F3&amp;","&amp;G3&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO Produits(libProduit, descProduit, refProduit, prixProduit, photoProduit, stock, idRubrique) VALUES ("poupée","poupée parfaite comme cadeau d'anniversaire ou de noël","h8d7g",15,"../IMG/poupee.png",150,1);</v>
+      </c>
+    </row>
+    <row r="4" ht="42.75">
+      <c r="A4" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="23">
+        <v>15</v>
+      </c>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23">
+        <v>70</v>
+      </c>
+      <c r="G4" s="23">
+        <f>VLOOKUP(H4,rubriques!$A$2:$C$6,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" s="23">
+        <v>3</v>
+      </c>
+      <c r="K4" t="str">
+        <f>"INSERT INTO Produits(libProduit, descProduit, refProduit, prixProduit, photoProduit, stock, idRubrique) VALUES ("""&amp;A4&amp;""","""&amp;B4&amp;""","""&amp;C4&amp;""","&amp;D4&amp;","""&amp;E4&amp;""","&amp;F4&amp;","&amp;G4&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO Produits(libProduit, descProduit, refProduit, prixProduit, photoProduit, stock, idRubrique) VALUES ("tournevis","Tournevis parfait pour vos tâches du quotidien","c8s23",15,"",70,3);</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="23">
+        <v>200</v>
+      </c>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23">
+        <v>25</v>
+      </c>
+      <c r="G5" s="23">
+        <f>VLOOKUP(H5,rubriques!$A$2:$C$6,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="23">
+        <v>4</v>
+      </c>
+      <c r="K5" t="str">
+        <f>"INSERT INTO Produits(libProduit, descProduit, refProduit, prixProduit, photoProduit, stock, idRubrique) VALUES ("""&amp;A5&amp;""","""&amp;B5&amp;""","""&amp;C5&amp;""","&amp;D5&amp;","""&amp;E5&amp;""","&amp;F5&amp;","&amp;G5&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO Produits(libProduit, descProduit, refProduit, prixProduit, photoProduit, stock, idRubrique) VALUES ("canapé","canapé très confortable","h8sdg",200,"",25,2);</v>
+      </c>
+    </row>
+    <row r="6" ht="42.75">
+      <c r="A6" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="23">
+        <v>345</v>
+      </c>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23">
+        <v>10</v>
+      </c>
+      <c r="G6" s="23">
+        <f>VLOOKUP(H6,rubriques!$A$2:$C$6,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="I6" s="23">
+        <v>5</v>
+      </c>
+      <c r="K6" t="str">
+        <f>"INSERT INTO Produits(libProduit, descProduit, refProduit, prixProduit, photoProduit, stock, idRubrique) VALUES ("""&amp;A6&amp;""","""&amp;B6&amp;""","""&amp;C6&amp;""","&amp;D6&amp;","""&amp;E6&amp;""","&amp;F6&amp;","&amp;G6&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO Produits(libProduit, descProduit, refProduit, prixProduit, photoProduit, stock, idRubrique) VALUES ("machine à laver","machine à laver parfaite pour vos vêtements","d8g3d",345,"",10,4);</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -1007,8 +1690,58 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="14.921875"/>
+    <col bestFit="1" min="2" max="2" width="12.57421875"/>
+    <col bestFit="1" min="4" max="4" width="59.2109375"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"INSERT INTO Fournisseurs(nomFournisseur) VALUES ("""&amp;A2&amp;""");"</f>
+        <v xml:space="preserve">INSERT INTO Fournisseurs(nomFournisseur) VALUES ("SuperElectro");</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2</v>
+      </c>
+      <c r="D3" t="str">
+        <f>"INSERT INTO Fournisseurs(nomFournisseur) VALUES ("""&amp;A3&amp;""");"</f>
+        <v xml:space="preserve">INSERT INTO Fournisseurs(nomFournisseur) VALUES ("SuperMaison");</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="10">
+        <v>3</v>
+      </c>
+      <c r="D4" t="str">
+        <f>"INSERT INTO Fournisseurs(nomFournisseur) VALUES ("""&amp;A4&amp;""");"</f>
+        <v xml:space="preserve">INSERT INTO Fournisseurs(nomFournisseur) VALUES ("SuperJouets");</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -1024,7 +1757,148 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="8.8515625"/>
+    <col bestFit="1" min="2" max="2" width="14.140625"/>
+    <col bestFit="1" min="3" max="3" width="12.57421875"/>
+    <col bestFit="1" min="4" max="4" width="14.921875"/>
+    <col bestFit="1" min="5" max="5" width="7.921875"/>
+    <col bestFit="1" min="7" max="7" width="50.421875"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="10">
+        <f>VLOOKUP(B2,produits!$A$2:$I$6,9,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="10">
+        <f>VLOOKUP(D2,fournisseurs!$A$2:$B$4,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="10">
+        <v>1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>"INSERT INTO fourni(idProduit, idFournisseur) VALUES ("&amp;A2&amp;","&amp;C2&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO fourni(idProduit, idFournisseur) VALUES (1,2);</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="10">
+        <f>VLOOKUP(B3,produits!$A$2:$I$6,9,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="10">
+        <f>VLOOKUP(D3,fournisseurs!$A$2:$B$4,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="10">
+        <v>2</v>
+      </c>
+      <c r="G3" t="str">
+        <f>"INSERT INTO fourni(idProduit, idFournisseur) VALUES ("&amp;A3&amp;","&amp;C3&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO fourni(idProduit, idFournisseur) VALUES (2,3);</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10">
+        <f>VLOOKUP(B4,produits!$A$2:$I$6,9,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="10">
+        <f>VLOOKUP(D4,fournisseurs!$A$2:$B$4,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="10">
+        <v>3</v>
+      </c>
+      <c r="G4" t="str">
+        <f>"INSERT INTO fourni(idProduit, idFournisseur) VALUES ("&amp;A4&amp;","&amp;C4&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO fourni(idProduit, idFournisseur) VALUES (3,2);</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="10">
+        <f>VLOOKUP(B5,produits!$A$2:$I$6,9,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="10">
+        <f>VLOOKUP(D5,fournisseurs!$A$2:$B$4,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="10">
+        <v>4</v>
+      </c>
+      <c r="G5" t="str">
+        <f>"INSERT INTO fourni(idProduit, idFournisseur) VALUES ("&amp;A5&amp;","&amp;C5&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO fourni(idProduit, idFournisseur) VALUES (4,2);</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10">
+        <f>VLOOKUP(B6,produits!$A$2:$I$6,9,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="10">
+        <f>VLOOKUP(D6,fournisseurs!$A$2:$B$4,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" s="10">
+        <v>5</v>
+      </c>
+      <c r="G6" t="str">
+        <f>"INSERT INTO fourni(idProduit, idFournisseur) VALUES ("&amp;A6&amp;","&amp;C6&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO fourni(idProduit, idFournisseur) VALUES (5,1);</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -1040,7 +1914,151 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="8.8515625"/>
+    <col bestFit="1" min="2" max="2" width="14.140625"/>
+    <col bestFit="1" min="3" max="3" width="19.28125"/>
+    <col bestFit="1" min="4" max="4" width="14.78125"/>
+    <col min="5" max="5" width="14.78125"/>
+    <col bestFit="1" min="6" max="6" width="9.921875"/>
+    <col min="7" max="7" width="9.921875"/>
+    <col bestFit="1" min="8" max="8" width="86.921875"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="26"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="23">
+        <f>VLOOKUP(B2,produits!$A$2:$I$6,9,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="23" t="str">
+        <f>VLOOKUP(D2,commandes!$A$2:$I$5,8,FALSE)</f>
+        <v xml:space="preserve">6 rue de béthune</v>
+      </c>
+      <c r="D2" s="23">
+        <v>7824938248</v>
+      </c>
+      <c r="E2" s="23">
+        <v>5</v>
+      </c>
+      <c r="F2" s="23">
+        <v>1</v>
+      </c>
+      <c r="G2" s="27"/>
+      <c r="H2" t="str">
+        <f>"INSERT INTO contient(idProduit, idCommande, quantiteProduit) VALUES ("&amp;A2&amp;","&amp;C2&amp;","&amp;E2&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO contient(idProduit, idCommande, quantiteProduit) VALUES (4,6 rue de béthune,5);</v>
+      </c>
+      <c r="I2" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="23">
+        <f>VLOOKUP(B3,produits!$A$2:$I$6,9,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="23" t="str">
+        <f>VLOOKUP(D3,commandes!$A$2:$I$5,8,FALSE)</f>
+        <v xml:space="preserve">740 rue des monts</v>
+      </c>
+      <c r="D3" s="23">
+        <v>9854673485</v>
+      </c>
+      <c r="E3" s="23">
+        <v>5</v>
+      </c>
+      <c r="F3" s="23">
+        <v>2</v>
+      </c>
+      <c r="G3" s="27"/>
+      <c r="H3" t="str">
+        <f>"INSERT INTO contient(idProduit, idCommande, quantiteProduit) VALUES ("&amp;A3&amp;","&amp;C3&amp;","&amp;E3&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO contient(idProduit, idCommande, quantiteProduit) VALUES (1,740 rue des monts,5);</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="23">
+        <f>VLOOKUP(B4,produits!$A$2:$I$6,9,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="23" t="str">
+        <f>VLOOKUP(D4,commandes!$A$2:$I$5,8,FALSE)</f>
+        <v xml:space="preserve">104 rue d'aire</v>
+      </c>
+      <c r="D4" s="23">
+        <v>1579875647</v>
+      </c>
+      <c r="E4" s="23">
+        <v>2</v>
+      </c>
+      <c r="F4" s="23">
+        <v>3</v>
+      </c>
+      <c r="G4" s="27"/>
+      <c r="H4" t="str">
+        <f>"INSERT INTO contient(idProduit, idCommande, quantiteProduit) VALUES ("&amp;A4&amp;","&amp;C4&amp;","&amp;E4&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO contient(idProduit, idCommande, quantiteProduit) VALUES (5,104 rue d'aire,2);</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="23">
+        <f>VLOOKUP(B5,produits!$A$2:$I$6,9,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="23" t="str">
+        <f>VLOOKUP(D5,commandes!$A$2:$I$5,8,FALSE)</f>
+        <v xml:space="preserve">2 rue de la préfecture</v>
+      </c>
+      <c r="D5" s="23">
+        <v>4723541584</v>
+      </c>
+      <c r="E5" s="23">
+        <v>25</v>
+      </c>
+      <c r="F5" s="23">
+        <v>4</v>
+      </c>
+      <c r="G5" s="27"/>
+      <c r="H5" t="str">
+        <f>"INSERT INTO contient(idProduit, idCommande, quantiteProduit) VALUES ("&amp;A5&amp;","&amp;C5&amp;","&amp;E5&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO contient(idProduit, idCommande, quantiteProduit) VALUES (2,2 rue de la préfecture,25);</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -1055,8 +2073,244 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="4" max="4" width="34.28125"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="23">
+        <v>20</v>
+      </c>
+      <c r="B2" s="23">
+        <v>1</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"INSERT INTO Tva(tauxTva) VALUES ("&amp;A2&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO Tva(tauxTva) VALUES (20);</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="23">
+        <v>10</v>
+      </c>
+      <c r="B3" s="23">
+        <v>2</v>
+      </c>
+      <c r="D3" t="str">
+        <f>"INSERT INTO Tva(tauxTva) VALUES ("&amp;A3&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO Tva(tauxTva) VALUES (10);</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="8.8515625"/>
+    <col bestFit="1" min="2" max="2" width="14.140625"/>
+    <col bestFit="1" min="3" max="3" width="5.421875"/>
+    <col bestFit="1" min="4" max="4" width="7.57421875"/>
+    <col bestFit="1" min="5" max="5" width="10.50390625"/>
+    <col bestFit="1" min="6" max="6" width="13.921875"/>
+    <col bestFit="1" min="7" max="7" width="10.28125"/>
+    <col bestFit="1" min="9" max="9" width="65.7109375"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="23">
+        <f>VLOOKUP(B2,produits!$A$2:$I$6,9,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="23">
+        <f>VLOOKUP(D2,tva!$A$2:$B$3,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="23">
+        <v>20</v>
+      </c>
+      <c r="E2" s="28">
+        <v>44893</v>
+      </c>
+      <c r="F2" s="28" t="str">
+        <f>TEXT(E2,"aaaa-mm-jj")</f>
+        <v>-11-jj</v>
+      </c>
+      <c r="G2" s="23">
+        <v>1</v>
+      </c>
+      <c r="I2" t="str">
+        <f>"INSERT INTO applique(idProduit, idTva, dateTva) VALUES ("&amp;A2&amp;","&amp;C2&amp;","""&amp;F2&amp;""");"</f>
+        <v xml:space="preserve">INSERT INTO applique(idProduit, idTva, dateTva) VALUES (1,1,"-11-jj");</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="23">
+        <f>VLOOKUP(B3,produits!$A$2:$I$6,9,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="23">
+        <f>VLOOKUP(D3,tva!$A$2:$B$3,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D3" s="23">
+        <v>10</v>
+      </c>
+      <c r="E3" s="28">
+        <v>44893</v>
+      </c>
+      <c r="F3" s="28" t="str">
+        <f>TEXT(E3,"aaaa-mm-jj")</f>
+        <v>-11-jj</v>
+      </c>
+      <c r="G3" s="23">
+        <v>2</v>
+      </c>
+      <c r="I3" t="str">
+        <f>"INSERT INTO applique(idProduit, idTva, dateTva) VALUES ("&amp;A3&amp;","&amp;C3&amp;","""&amp;F3&amp;""");"</f>
+        <v xml:space="preserve">INSERT INTO applique(idProduit, idTva, dateTva) VALUES (2,2,"-11-jj");</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="23">
+        <f>VLOOKUP(B4,produits!$A$2:$I$6,9,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="23">
+        <f>VLOOKUP(D4,tva!$A$2:$B$3,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D4" s="23">
+        <v>10</v>
+      </c>
+      <c r="E4" s="28">
+        <v>44893</v>
+      </c>
+      <c r="F4" s="28" t="str">
+        <f>TEXT(E4,"aaaa-mm-jj")</f>
+        <v>-11-jj</v>
+      </c>
+      <c r="G4" s="23">
+        <v>3</v>
+      </c>
+      <c r="I4" t="str">
+        <f>"INSERT INTO applique(idProduit, idTva, dateTva) VALUES ("&amp;A4&amp;","&amp;C4&amp;","""&amp;F4&amp;""");"</f>
+        <v xml:space="preserve">INSERT INTO applique(idProduit, idTva, dateTva) VALUES (3,2,"-11-jj");</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="23">
+        <f>VLOOKUP(B5,produits!$A$2:$I$6,9,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="23">
+        <f>VLOOKUP(D5,tva!$A$2:$B$3,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="23">
+        <v>20</v>
+      </c>
+      <c r="E5" s="28">
+        <v>44893</v>
+      </c>
+      <c r="F5" s="28" t="str">
+        <f>TEXT(E5,"aaaa-mm-jj")</f>
+        <v>-11-jj</v>
+      </c>
+      <c r="G5" s="23">
+        <v>4</v>
+      </c>
+      <c r="I5" t="str">
+        <f>"INSERT INTO applique(idProduit, idTva, dateTva) VALUES ("&amp;A5&amp;","&amp;C5&amp;","""&amp;F5&amp;""");"</f>
+        <v xml:space="preserve">INSERT INTO applique(idProduit, idTva, dateTva) VALUES (4,1,"-11-jj");</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="23">
+        <f>VLOOKUP(B6,produits!$A$2:$I$6,9,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="23">
+        <f>VLOOKUP(D6,tva!$A$2:$B$3,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="23">
+        <v>20</v>
+      </c>
+      <c r="E6" s="28">
+        <v>44893</v>
+      </c>
+      <c r="F6" s="28" t="str">
+        <f>TEXT(E6,"aaaa-mm-jj")</f>
+        <v>-11-jj</v>
+      </c>
+      <c r="G6" s="23">
+        <v>5</v>
+      </c>
+      <c r="I6" t="str">
+        <f>"INSERT INTO applique(idProduit, idTva, dateTva) VALUES ("&amp;A6&amp;","&amp;C6&amp;","""&amp;F6&amp;""");"</f>
+        <v xml:space="preserve">INSERT INTO applique(idProduit, idTva, dateTva) VALUES (5,1,"-11-jj");</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -1220,13 +2474,13 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D1" s="8"/>
@@ -1598,20 +2852,20 @@
   <cols>
     <col bestFit="1" min="1" max="1" width="12.140625"/>
     <col bestFit="1" min="2" max="2" width="10.140625"/>
-    <col bestFit="1" min="4" max="4" width="59.7109375"/>
+    <col bestFit="1" min="4" max="4" width="60.50390625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>48</v>
       </c>
       <c r="C1" s="8"/>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" t="s">
+      <c r="A2" s="10" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="13">
@@ -1619,12 +2873,12 @@
       </c>
       <c r="C2" s="14"/>
       <c r="D2" t="str">
-        <f>"INSERT INTO CategoriesClient(libCatClient) VALUES ("""&amp;A2&amp;""");"</f>
-        <v xml:space="preserve">INSERT INTO CategoriesClient(libCatClient) VALUES ("Particulier");</v>
+        <f>"INSERT INTO CategoriesClients(libCatClient) VALUES ("""&amp;A2&amp;""");"</f>
+        <v xml:space="preserve">INSERT INTO CategoriesClients(libCatClient) VALUES ("Particulier");</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" t="s">
+      <c r="A3" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B3" s="13">
@@ -1632,8 +2886,8 @@
       </c>
       <c r="C3" s="14"/>
       <c r="D3" t="str">
-        <f>"INSERT INTO CategoriesClient(libCatClient) VALUES ("""&amp;A3&amp;""");"</f>
-        <v xml:space="preserve">INSERT INTO CategoriesClient(libCatClient) VALUES ("Professionnel");</v>
+        <f>"INSERT INTO CategoriesClients(libCatClient) VALUES ("""&amp;A3&amp;""");"</f>
+        <v xml:space="preserve">INSERT INTO CategoriesClients(libCatClient) VALUES ("Professionnel");</v>
       </c>
     </row>
   </sheetData>
@@ -1659,37 +2913,37 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="9" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="10">
+        <v>2</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="10">
         <f>VLOOKUP(D2,categoriesClients!$A$2:$B$3,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="10">
         <v>1</v>
       </c>
       <c r="G2" t="str">
@@ -1698,20 +2952,20 @@
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="10">
         <f>VLOOKUP(D3,categoriesClients!$A$2:$B$3,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="10">
         <v>2</v>
       </c>
       <c r="G3" t="str">
@@ -1720,20 +2974,20 @@
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4">
+      <c r="A4" s="10">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="10">
         <f>VLOOKUP(D4,categoriesClients!$A$2:$B$3,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="10">
         <v>3</v>
       </c>
       <c r="G4" t="str">
@@ -1742,20 +2996,20 @@
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5">
+      <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="10">
         <f>VLOOKUP(D5,categoriesClients!$A$2:$B$3,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="10">
         <v>4</v>
       </c>
       <c r="G5" t="str">
@@ -1778,8 +3032,194 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="14.78125"/>
+    <col bestFit="1" min="2" max="2" width="14.7109375"/>
+    <col bestFit="1" min="3" max="3" width="20.921875"/>
+    <col bestFit="1" min="4" max="4" width="7.421875"/>
+    <col bestFit="1" min="5" max="5" width="14.140625"/>
+    <col bestFit="1" min="6" max="6" width="8.2109375"/>
+    <col bestFit="1" min="7" max="7" width="9.3515625"/>
+    <col bestFit="1" min="8" max="8" width="19.28125"/>
+    <col bestFit="1" min="9" max="9" width="12.00390625"/>
+    <col bestFit="1" min="11" max="11" width="105.640625"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="10">
+        <v>1579875647</v>
+      </c>
+      <c r="B2" s="16">
+        <v>44889</v>
+      </c>
+      <c r="C2" s="16" t="str">
+        <f>TEXT(B2,"aaaa-mm-jj")</f>
+        <v>-11-jj</v>
+      </c>
+      <c r="D2" s="10" t="e">
+        <f>VLOOKUP(F2,clients!$A$2:$E$5,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E2" s="10">
+        <v>1</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="10">
+        <f>VLOOKUP(H2,adresses!$A$2:$G$8,6,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="10">
+        <v>1</v>
+      </c>
+      <c r="K2" t="str">
+        <f>"INSERT INTO Commandes(numCommande, dateCommande, idClient, idAdresse) VALUES ("""&amp;A2&amp;""","""&amp;C2&amp;""","&amp;E2&amp;","&amp;G2&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO Commandes(numCommande, dateCommande, idClient, idAdresse) VALUES ("1579875647","-11-jj",1,5);</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="10">
+        <v>7824938248</v>
+      </c>
+      <c r="B3" s="16">
+        <v>44392</v>
+      </c>
+      <c r="C3" s="16" t="str">
+        <f>TEXT(B3,"aaaa-mm-jj")</f>
+        <v>-07-jj</v>
+      </c>
+      <c r="D3" s="10" t="e">
+        <f>VLOOKUP(F3,clients!$A$2:$E$5,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E3" s="10">
+        <v>2</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="10">
+        <f>VLOOKUP(H3,adresses!$A$2:$G$8,6,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="10">
+        <v>2</v>
+      </c>
+      <c r="K3" t="str">
+        <f>"INSERT INTO Commandes(numCommande, dateCommande, idClient, idAdresse) VALUES ("""&amp;A3&amp;""","""&amp;C3&amp;""","&amp;E3&amp;","&amp;G3&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO Commandes(numCommande, dateCommande, idClient, idAdresse) VALUES ("7824938248","-07-jj",2,3);</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="10">
+        <v>9854673485</v>
+      </c>
+      <c r="B4" s="16">
+        <v>43958</v>
+      </c>
+      <c r="C4" s="16" t="str">
+        <f>TEXT(B4,"aaaa-mm-jj")</f>
+        <v>-05-jj</v>
+      </c>
+      <c r="D4" s="10" t="e">
+        <f>VLOOKUP(F4,clients!$A$2:$E$5,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E4" s="10">
+        <v>3</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="10">
+        <f>VLOOKUP(H4,adresses!$A$2:$G$8,6,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="10">
+        <v>3</v>
+      </c>
+      <c r="K4" t="str">
+        <f>"INSERT INTO Commandes(numCommande, dateCommande, idClient, idAdresse) VALUES ("""&amp;A4&amp;""","""&amp;C4&amp;""","&amp;E4&amp;","&amp;G4&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO Commandes(numCommande, dateCommande, idClient, idAdresse) VALUES ("9854673485","-05-jj",3,7);</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="10">
+        <v>4723541584</v>
+      </c>
+      <c r="B5" s="16">
+        <v>44608</v>
+      </c>
+      <c r="C5" s="16" t="str">
+        <f>TEXT(B5,"aaaa-mm-jj")</f>
+        <v>-02-jj</v>
+      </c>
+      <c r="D5" s="10" t="e">
+        <f>VLOOKUP(F5,clients!$A$2:$E$5,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E5" s="10">
+        <v>4</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="10">
+        <f>VLOOKUP(H5,adresses!$A$2:$G$8,6,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="10">
+        <v>4</v>
+      </c>
+      <c r="K5" t="str">
+        <f>"INSERT INTO Commandes(numCommande, dateCommande, idClient, idAdresse) VALUES ("""&amp;A5&amp;""","""&amp;C5&amp;""","&amp;E5&amp;","&amp;G5&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO Commandes(numCommande, dateCommande, idClient, idAdresse) VALUES ("4723541584","-02-jj",4,2);</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -1794,8 +3234,178 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="9.3515625"/>
+    <col bestFit="1" min="2" max="2" width="19.28125"/>
+    <col bestFit="1" min="3" max="3" width="12.421875"/>
+    <col bestFit="1" min="4" max="4" width="14.78125"/>
+    <col bestFit="1" min="5" max="5" width="12.3515625"/>
+    <col bestFit="1" min="6" max="6" width="18.57421875"/>
+    <col bestFit="1" min="7" max="7" width="15.8515625"/>
+    <col bestFit="1" min="8" max="8" width="6.50390625"/>
+    <col bestFit="1" min="10" max="10" width="92.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="19">
+        <f>VLOOKUP(B2,adresses!$A$2:$G$8,6,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="19" t="str">
+        <f>VLOOKUP(D2,commandes!$A$2:$I$5,8,FALSE)</f>
+        <v xml:space="preserve">6 rue de béthune</v>
+      </c>
+      <c r="D2" s="19">
+        <v>7824938248</v>
+      </c>
+      <c r="E2" s="20">
+        <v>44397</v>
+      </c>
+      <c r="F2" s="20" t="str">
+        <f>TEXT(E2,"aaaa-mm-jj")</f>
+        <v>-07-jj</v>
+      </c>
+      <c r="G2" s="19">
+        <v>5</v>
+      </c>
+      <c r="H2" s="19">
+        <v>1</v>
+      </c>
+      <c r="J2" t="str">
+        <f>"INSERT INTO livre(idAdresse, idCommande, dateLivraison, quantiteLivraison) VALUES ("&amp;A2&amp;","&amp;C2&amp;","""&amp;F2&amp;""","&amp;G2&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO livre(idAdresse, idCommande, dateLivraison, quantiteLivraison) VALUES (3,6 rue de béthune,"-07-jj",5);</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="19">
+        <f>VLOOKUP(B3,adresses!$A$2:$G$8,6,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="19" t="str">
+        <f>VLOOKUP(D3,commandes!$A$2:$I$5,8,FALSE)</f>
+        <v xml:space="preserve">104 rue d'aire</v>
+      </c>
+      <c r="D3" s="19">
+        <v>1579875647</v>
+      </c>
+      <c r="E3" s="20">
+        <v>44900</v>
+      </c>
+      <c r="F3" s="20" t="str">
+        <f>TEXT(E3,"aaaa-mm-jj")</f>
+        <v>-12-jj</v>
+      </c>
+      <c r="G3" s="19">
+        <v>2</v>
+      </c>
+      <c r="H3" s="19">
+        <v>2</v>
+      </c>
+      <c r="J3" t="str">
+        <f>"INSERT INTO livre(idAdresse, idCommande, dateLivraison, quantiteLivraison) VALUES ("&amp;A3&amp;","&amp;C3&amp;","""&amp;F3&amp;""","&amp;G3&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO livre(idAdresse, idCommande, dateLivraison, quantiteLivraison) VALUES (5,104 rue d'aire,"-12-jj",2);</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="19">
+        <f>VLOOKUP(B4,adresses!$A$2:$G$8,6,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="19" t="str">
+        <f>VLOOKUP(D4,commandes!$A$2:$I$5,8,FALSE)</f>
+        <v xml:space="preserve">2 rue de la préfecture</v>
+      </c>
+      <c r="D4" s="19">
+        <v>4723541584</v>
+      </c>
+      <c r="E4" s="20">
+        <v>44620</v>
+      </c>
+      <c r="F4" s="20" t="str">
+        <f>TEXT(E4,"aaaa-mm-jj")</f>
+        <v>-02-jj</v>
+      </c>
+      <c r="G4" s="19">
+        <v>25</v>
+      </c>
+      <c r="H4" s="19">
+        <v>3</v>
+      </c>
+      <c r="J4" t="str">
+        <f>"INSERT INTO livre(idAdresse, idCommande, dateLivraison, quantiteLivraison) VALUES ("&amp;A4&amp;","&amp;C4&amp;","""&amp;F4&amp;""","&amp;G4&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO livre(idAdresse, idCommande, dateLivraison, quantiteLivraison) VALUES (2,2 rue de la préfecture,"-02-jj",25);</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="19">
+        <f>VLOOKUP(B5,adresses!$A$2:$G$8,6,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="19" t="str">
+        <f>VLOOKUP(D5,commandes!$A$2:$I$5,8,FALSE)</f>
+        <v xml:space="preserve">740 rue des monts</v>
+      </c>
+      <c r="D5" s="19">
+        <v>9854673485</v>
+      </c>
+      <c r="E5" s="20">
+        <v>43978</v>
+      </c>
+      <c r="F5" s="20" t="str">
+        <f>TEXT(E5,"aaaa-mm-jj")</f>
+        <v>-05-jj</v>
+      </c>
+      <c r="G5" s="19">
+        <v>5</v>
+      </c>
+      <c r="H5" s="19">
+        <v>4</v>
+      </c>
+      <c r="J5" t="str">
+        <f>"INSERT INTO livre(idAdresse, idCommande, dateLivraison, quantiteLivraison) VALUES ("&amp;A5&amp;","&amp;C5&amp;","""&amp;F5&amp;""","&amp;G5&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO livre(idAdresse, idCommande, dateLivraison, quantiteLivraison) VALUES (7,740 rue des monts,"-05-jj",5);</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -1811,7 +3421,45 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="13.00390625"/>
+    <col bestFit="1" min="2" max="2" width="11.8515625"/>
+    <col bestFit="1" min="4" max="4" width="54.7109375"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"INSERT INTO Reglements(typePaiement) VALUES ("""&amp;A2&amp;""");"</f>
+        <v xml:space="preserve">INSERT INTO Reglements(typePaiement) VALUES ("Différé");</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2</v>
+      </c>
+      <c r="D3" t="str">
+        <f>"INSERT INTO Reglements(typePaiement) VALUES ("""&amp;A3&amp;""");"</f>
+        <v xml:space="preserve">INSERT INTO Reglements(typePaiement) VALUES ("Comptant");</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>

</xml_diff>